<commit_message>
update files to 20230722160703
</commit_message>
<xml_diff>
--- a/phase/tmc_img/file hàng loat/tmc_laz_2.xlsx
+++ b/phase/tmc_img/file hàng loat/tmc_laz_2.xlsx
@@ -5,13 +5,13 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\bash-script\phase\tmc_img\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\bash-script\phase\tmc_img\file hàng loat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACAE6CD-4B47-4323-BA16-DD6A92CBEE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C17F420-90CF-4B38-A790-26041B68DF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="MD5" workbookHashValue="QoBlpy4ORMvn9wwEqwBNPw==" workbookSaltValue="aZ/9ucYC3aaGUkwrnAfqnQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INDEX" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Xemôhình_hide" sheetId="3" state="hidden" r:id="rId3"/>
     <sheet name="global_hide" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2122,9 +2122,6 @@
     <t>Xe mô hình Tomica Regular No.89 Lamborghini Sian</t>
   </si>
   <si>
-    <t>Xe mô hình Tomica No.31 Toyota Camry Sports Unmarked Police Car</t>
-  </si>
-  <si>
     <t>Xe mô hình Tomica Regular No.15 Hummer V2</t>
   </si>
   <si>
@@ -2874,6 +2871,9 @@
   </si>
   <si>
     <t>https://i.imgur.com/e8onpZs.jpg</t>
+  </si>
+  <si>
+    <t>Xe mô hình Tomica Regular No.31 Toyota Camry Sports Unmarked Police Car</t>
   </si>
 </sst>
 </file>
@@ -5457,9 +5457,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BG30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BF19" sqref="BF19"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6211,7 +6211,7 @@
         <v>671</v>
       </c>
       <c r="E5" s="243" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>672</v>
@@ -6232,10 +6232,10 @@
         <v>218</v>
       </c>
       <c r="BA5" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="BC5" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD5" s="3">
         <v>0.5</v>
@@ -6255,7 +6255,7 @@
         <v>674</v>
       </c>
       <c r="E6" s="243" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>672</v>
@@ -6267,7 +6267,7 @@
         <v>224</v>
       </c>
       <c r="AF6" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="AK6" s="6" t="s">
         <v>280</v>
@@ -6276,10 +6276,10 @@
         <v>218</v>
       </c>
       <c r="BA6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="BC6" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD6" s="3">
         <v>0.5</v>
@@ -6299,7 +6299,7 @@
         <v>675</v>
       </c>
       <c r="E7" s="243" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="Q7" s="6" t="s">
         <v>672</v>
@@ -6311,7 +6311,7 @@
         <v>224</v>
       </c>
       <c r="AF7" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="AK7" s="6" t="s">
         <v>280</v>
@@ -6320,10 +6320,10 @@
         <v>218</v>
       </c>
       <c r="BA7" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="BC7" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD7" s="3">
         <v>0.5</v>
@@ -6343,7 +6343,7 @@
         <v>676</v>
       </c>
       <c r="E8" s="243" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>672</v>
@@ -6355,7 +6355,7 @@
         <v>224</v>
       </c>
       <c r="AF8" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="AK8" s="6" t="s">
         <v>280</v>
@@ -6364,10 +6364,10 @@
         <v>218</v>
       </c>
       <c r="BA8" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC8" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD8" s="3">
         <v>0.5</v>
@@ -6387,7 +6387,7 @@
         <v>677</v>
       </c>
       <c r="E9" s="243" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="Q9" s="6" t="s">
         <v>672</v>
@@ -6399,7 +6399,7 @@
         <v>224</v>
       </c>
       <c r="AF9" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="AK9" s="6" t="s">
         <v>280</v>
@@ -6408,10 +6408,10 @@
         <v>218</v>
       </c>
       <c r="BA9" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC9" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD9" s="3">
         <v>0.5</v>
@@ -6431,7 +6431,7 @@
         <v>678</v>
       </c>
       <c r="E10" s="243" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="Q10" s="6" t="s">
         <v>672</v>
@@ -6443,7 +6443,7 @@
         <v>224</v>
       </c>
       <c r="AF10" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="AK10" s="6" t="s">
         <v>280</v>
@@ -6452,10 +6452,10 @@
         <v>218</v>
       </c>
       <c r="BA10" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC10" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD10" s="3">
         <v>0.5</v>
@@ -6475,7 +6475,7 @@
         <v>679</v>
       </c>
       <c r="E11" s="243" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="Q11" s="6" t="s">
         <v>672</v>
@@ -6487,7 +6487,7 @@
         <v>224</v>
       </c>
       <c r="AF11" s="244" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="AK11" s="6" t="s">
         <v>280</v>
@@ -6496,10 +6496,10 @@
         <v>218</v>
       </c>
       <c r="BA11" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="BC11" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD11" s="3">
         <v>0.5</v>
@@ -6519,7 +6519,7 @@
         <v>680</v>
       </c>
       <c r="E12" s="243" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="Q12" s="6" t="s">
         <v>672</v>
@@ -6531,7 +6531,7 @@
         <v>224</v>
       </c>
       <c r="AF12" s="244" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="AK12" s="6" t="s">
         <v>280</v>
@@ -6540,10 +6540,10 @@
         <v>218</v>
       </c>
       <c r="BA12" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC12" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD12" s="3">
         <v>0.5</v>
@@ -6563,7 +6563,7 @@
         <v>681</v>
       </c>
       <c r="E13" s="243" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="Q13" s="6" t="s">
         <v>672</v>
@@ -6575,7 +6575,7 @@
         <v>224</v>
       </c>
       <c r="AF13" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="AK13" s="6" t="s">
         <v>280</v>
@@ -6584,10 +6584,10 @@
         <v>218</v>
       </c>
       <c r="BA13" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC13" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD13" s="3">
         <v>0.5</v>
@@ -6607,7 +6607,7 @@
         <v>682</v>
       </c>
       <c r="E14" s="243" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="Q14" s="6" t="s">
         <v>672</v>
@@ -6619,7 +6619,7 @@
         <v>224</v>
       </c>
       <c r="AF14" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="AK14" s="6" t="s">
         <v>280</v>
@@ -6628,10 +6628,10 @@
         <v>218</v>
       </c>
       <c r="BA14" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="BC14" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD14" s="3">
         <v>0.5</v>
@@ -6651,7 +6651,7 @@
         <v>683</v>
       </c>
       <c r="E15" s="243" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="Q15" s="6" t="s">
         <v>672</v>
@@ -6663,7 +6663,7 @@
         <v>224</v>
       </c>
       <c r="AF15" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="AK15" s="6" t="s">
         <v>280</v>
@@ -6672,10 +6672,10 @@
         <v>218</v>
       </c>
       <c r="BA15" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC15" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD15" s="3">
         <v>0.5</v>
@@ -6695,7 +6695,7 @@
         <v>684</v>
       </c>
       <c r="E16" s="243" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="Q16" s="6" t="s">
         <v>672</v>
@@ -6707,7 +6707,7 @@
         <v>224</v>
       </c>
       <c r="AF16" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="AK16" s="6" t="s">
         <v>280</v>
@@ -6716,10 +6716,10 @@
         <v>218</v>
       </c>
       <c r="BA16" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC16" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD16" s="3">
         <v>0.5</v>
@@ -6739,7 +6739,7 @@
         <v>685</v>
       </c>
       <c r="E17" s="243" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="Q17" s="6" t="s">
         <v>672</v>
@@ -6751,7 +6751,7 @@
         <v>224</v>
       </c>
       <c r="AF17" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="AK17" s="6" t="s">
         <v>280</v>
@@ -6760,10 +6760,10 @@
         <v>218</v>
       </c>
       <c r="BA17" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC17" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD17" s="3">
         <v>0.5</v>
@@ -6783,7 +6783,7 @@
         <v>686</v>
       </c>
       <c r="E18" s="243" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="Q18" s="6" t="s">
         <v>672</v>
@@ -6795,7 +6795,7 @@
         <v>224</v>
       </c>
       <c r="AF18" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="AK18" s="6" t="s">
         <v>280</v>
@@ -6804,10 +6804,10 @@
         <v>218</v>
       </c>
       <c r="BA18" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC18" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD18" s="3">
         <v>0.5</v>
@@ -6824,10 +6824,10 @@
     </row>
     <row r="19" spans="3:59" ht="20" customHeight="1">
       <c r="C19" s="245" t="s">
-        <v>687</v>
+        <v>754</v>
       </c>
       <c r="E19" s="243" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="Q19" s="6" t="s">
         <v>672</v>
@@ -6839,7 +6839,7 @@
         <v>224</v>
       </c>
       <c r="AF19" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="AK19" s="6" t="s">
         <v>280</v>
@@ -6848,10 +6848,10 @@
         <v>218</v>
       </c>
       <c r="BA19" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC19" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD19" s="3">
         <v>0.5</v>
@@ -6868,10 +6868,10 @@
     </row>
     <row r="20" spans="3:59" ht="20" customHeight="1">
       <c r="C20" s="245" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E20" s="243" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="Q20" s="6" t="s">
         <v>672</v>
@@ -6883,7 +6883,7 @@
         <v>224</v>
       </c>
       <c r="AF20" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="AK20" s="6" t="s">
         <v>280</v>
@@ -6892,10 +6892,10 @@
         <v>218</v>
       </c>
       <c r="BA20" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC20" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD20" s="3">
         <v>0.5</v>
@@ -6912,10 +6912,10 @@
     </row>
     <row r="21" spans="3:59" ht="20" customHeight="1">
       <c r="C21" s="245" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E21" s="243" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="Q21" s="6" t="s">
         <v>672</v>
@@ -6927,7 +6927,7 @@
         <v>224</v>
       </c>
       <c r="AF21" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="AK21" s="6" t="s">
         <v>280</v>
@@ -6936,10 +6936,10 @@
         <v>218</v>
       </c>
       <c r="BA21" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC21" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD21" s="3">
         <v>0.5</v>
@@ -6956,10 +6956,10 @@
     </row>
     <row r="22" spans="3:59" ht="20" customHeight="1">
       <c r="C22" s="245" t="s">
+        <v>744</v>
+      </c>
+      <c r="E22" s="243" t="s">
         <v>745</v>
-      </c>
-      <c r="E22" s="243" t="s">
-        <v>746</v>
       </c>
       <c r="Q22" s="6" t="s">
         <v>672</v>
@@ -6971,7 +6971,7 @@
         <v>224</v>
       </c>
       <c r="AF22" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="AK22" s="6" t="s">
         <v>280</v>
@@ -6980,10 +6980,10 @@
         <v>218</v>
       </c>
       <c r="BA22" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC22" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD22" s="3">
         <v>0.5</v>
@@ -7000,10 +7000,10 @@
     </row>
     <row r="23" spans="3:59" ht="20" customHeight="1">
       <c r="C23" s="245" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E23" s="243" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="Q23" s="6" t="s">
         <v>672</v>
@@ -7015,7 +7015,7 @@
         <v>224</v>
       </c>
       <c r="AF23" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="AK23" s="6" t="s">
         <v>280</v>
@@ -7024,10 +7024,10 @@
         <v>218</v>
       </c>
       <c r="BA23" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC23" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD23" s="3">
         <v>0.5</v>
@@ -7044,10 +7044,10 @@
     </row>
     <row r="24" spans="3:59" ht="20" customHeight="1">
       <c r="C24" s="245" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E24" s="243" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="Q24" s="6" t="s">
         <v>672</v>
@@ -7059,7 +7059,7 @@
         <v>224</v>
       </c>
       <c r="AF24" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="AK24" s="6" t="s">
         <v>280</v>
@@ -7068,10 +7068,10 @@
         <v>218</v>
       </c>
       <c r="BA24" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC24" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD24" s="3">
         <v>0.5</v>
@@ -7088,10 +7088,10 @@
     </row>
     <row r="25" spans="3:59" ht="20" customHeight="1">
       <c r="C25" s="245" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E25" s="243" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="Q25" s="6" t="s">
         <v>672</v>
@@ -7103,7 +7103,7 @@
         <v>224</v>
       </c>
       <c r="AF25" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="AK25" s="6" t="s">
         <v>280</v>
@@ -7112,10 +7112,10 @@
         <v>218</v>
       </c>
       <c r="BA25" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC25" s="245" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="BD25" s="3">
         <v>0.5</v>
@@ -7132,10 +7132,10 @@
     </row>
     <row r="26" spans="3:59" ht="20" customHeight="1">
       <c r="C26" s="245" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E26" s="243" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>672</v>
@@ -7147,7 +7147,7 @@
         <v>224</v>
       </c>
       <c r="AF26" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="AK26" s="6" t="s">
         <v>280</v>
@@ -7156,10 +7156,10 @@
         <v>218</v>
       </c>
       <c r="BA26" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC26" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD26" s="3">
         <v>0.5</v>
@@ -7176,10 +7176,10 @@
     </row>
     <row r="27" spans="3:59" ht="20" customHeight="1">
       <c r="C27" s="245" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="Q27" s="6" t="s">
         <v>672</v>
@@ -7191,7 +7191,7 @@
         <v>224</v>
       </c>
       <c r="AF27" s="6" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="AK27" s="6" t="s">
         <v>280</v>
@@ -7200,10 +7200,10 @@
         <v>218</v>
       </c>
       <c r="BA27" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC27" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD27" s="3">
         <v>0.5</v>
@@ -7220,10 +7220,10 @@
     </row>
     <row r="28" spans="3:59" ht="20" customHeight="1">
       <c r="C28" s="245" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="Q28" s="6" t="s">
         <v>672</v>
@@ -7235,7 +7235,7 @@
         <v>224</v>
       </c>
       <c r="AF28" s="6" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="AK28" s="6" t="s">
         <v>280</v>
@@ -7244,10 +7244,10 @@
         <v>218</v>
       </c>
       <c r="BA28" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC28" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD28" s="3">
         <v>0.5</v>
@@ -7264,10 +7264,10 @@
     </row>
     <row r="29" spans="3:59" ht="20" customHeight="1">
       <c r="C29" s="245" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="Q29" s="6" t="s">
         <v>672</v>
@@ -7279,7 +7279,7 @@
         <v>224</v>
       </c>
       <c r="AF29" s="6" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="AK29" s="6" t="s">
         <v>280</v>
@@ -7288,10 +7288,10 @@
         <v>218</v>
       </c>
       <c r="BA29" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="BC29" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD29" s="3">
         <v>0.5</v>
@@ -7308,10 +7308,10 @@
     </row>
     <row r="30" spans="3:59" ht="20" customHeight="1">
       <c r="C30" s="245" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>672</v>
@@ -7323,7 +7323,7 @@
         <v>224</v>
       </c>
       <c r="AF30" s="6" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="AK30" s="6" t="s">
         <v>280</v>
@@ -7332,10 +7332,10 @@
         <v>218</v>
       </c>
       <c r="BA30" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="BC30" s="245" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="BD30" s="3">
         <v>0.5</v>

</xml_diff>